<commit_message>
Decrease voltage variable size to U8
</commit_message>
<xml_diff>
--- a/Calculation algorithm.xlsx
+++ b/Calculation algorithm.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
@@ -12,7 +12,7 @@
     <sheet name="XZ circle Y linear path" sheetId="2" r:id="rId3"/>
     <sheet name="ZX elliptical Y sinus path" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -1000,6 +1000,16 @@
     <xf numFmtId="164" fontId="0" fillId="9" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1045,19 +1055,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -1347,11 +1347,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="92087424"/>
-        <c:axId val="92088960"/>
+        <c:axId val="222249984"/>
+        <c:axId val="220691776"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="92087424"/>
+        <c:axId val="222249984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1362,7 +1362,7 @@
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92088960"/>
+        <c:crossAx val="220691776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1370,7 +1370,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="92088960"/>
+        <c:axId val="220691776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -1383,7 +1383,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92087424"/>
+        <c:crossAx val="222249984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
@@ -1684,11 +1684,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="72554368"/>
-        <c:axId val="88761856"/>
+        <c:axId val="224412800"/>
+        <c:axId val="224413376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="72554368"/>
+        <c:axId val="224412800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10"/>
@@ -1700,12 +1700,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88761856"/>
+        <c:crossAx val="224413376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="88761856"/>
+        <c:axId val="224413376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10"/>
@@ -1718,7 +1718,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72554368"/>
+        <c:crossAx val="224412800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2018,11 +2018,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="90920448"/>
-        <c:axId val="90528384"/>
+        <c:axId val="224415104"/>
+        <c:axId val="224415680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="90920448"/>
+        <c:axId val="224415104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10"/>
@@ -2034,12 +2034,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90528384"/>
+        <c:crossAx val="224415680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="90528384"/>
+        <c:axId val="224415680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10"/>
@@ -2052,7 +2052,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90920448"/>
+        <c:crossAx val="224415104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2181,9 +2181,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2221,7 +2221,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -2293,7 +2293,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2469,7 +2469,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:R15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2486,31 +2488,31 @@
       <c r="C2" s="2">
         <v>45</v>
       </c>
-      <c r="E2" s="87" t="s">
+      <c r="E2" s="91" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
-      <c r="H2" s="92" t="s">
+      <c r="F2" s="103"/>
+      <c r="G2" s="103"/>
+      <c r="H2" s="96" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="93"/>
-      <c r="J2" s="99" t="s">
+      <c r="I2" s="97"/>
+      <c r="J2" s="103" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="99"/>
-      <c r="L2" s="88"/>
-      <c r="M2" s="87" t="s">
+      <c r="K2" s="103"/>
+      <c r="L2" s="92"/>
+      <c r="M2" s="91" t="s">
         <v>15</v>
       </c>
-      <c r="N2" s="88"/>
+      <c r="N2" s="92"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="4">
-        <v>135</v>
+        <v>101</v>
       </c>
       <c r="E3" s="20" t="s">
         <v>10</v>
@@ -2548,15 +2550,15 @@
         <v>5</v>
       </c>
       <c r="C4" s="4">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E4" s="13">
         <f>C9*COS(RADIANS(C2)) + C11*SIN(RADIANS(C2))</f>
-        <v>98.994949366116657</v>
+        <v>141.42135623730951</v>
       </c>
       <c r="F4" s="14">
         <f>C10</f>
-        <v>-85</v>
+        <v>-40</v>
       </c>
       <c r="G4" s="40">
         <f>-C9*SIN(RADIANS(C2)) + C11*COS(RADIANS(C2))</f>
@@ -2572,11 +2574,11 @@
       </c>
       <c r="J4" s="42">
         <f>E4*COS(H4) + G4*SIN(H4)</f>
-        <v>98.994949366116657</v>
+        <v>141.42135623730951</v>
       </c>
       <c r="K4" s="14">
         <f>F4</f>
-        <v>-85</v>
+        <v>-40</v>
       </c>
       <c r="L4" s="15">
         <f xml:space="preserve"> -E4*SIN(H4) + G4*COS(H4)</f>
@@ -2584,11 +2586,11 @@
       </c>
       <c r="M4" s="18">
         <f>J4-C5</f>
-        <v>58.994949366116657</v>
+        <v>101.42135623730951</v>
       </c>
       <c r="N4" s="19">
         <f>K4</f>
-        <v>-85</v>
+        <v>-40</v>
       </c>
     </row>
     <row r="5" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2604,21 +2606,21 @@
         <v>8</v>
       </c>
       <c r="C6" s="4">
-        <v>85</v>
-      </c>
-      <c r="E6" s="89" t="s">
+        <v>84</v>
+      </c>
+      <c r="E6" s="93" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="90"/>
-      <c r="G6" s="90"/>
-      <c r="H6" s="90"/>
-      <c r="I6" s="90"/>
-      <c r="J6" s="90"/>
-      <c r="K6" s="90"/>
-      <c r="L6" s="90"/>
-      <c r="M6" s="90"/>
-      <c r="N6" s="90"/>
-      <c r="O6" s="91"/>
+      <c r="F6" s="94"/>
+      <c r="G6" s="94"/>
+      <c r="H6" s="94"/>
+      <c r="I6" s="94"/>
+      <c r="J6" s="94"/>
+      <c r="K6" s="94"/>
+      <c r="L6" s="94"/>
+      <c r="M6" s="94"/>
+      <c r="N6" s="94"/>
+      <c r="O6" s="95"/>
       <c r="P6" s="38"/>
       <c r="Q6" s="38"/>
       <c r="R6" s="38"/>
@@ -2630,10 +2632,10 @@
       <c r="C7" s="6">
         <v>141</v>
       </c>
-      <c r="E7" s="94" t="s">
+      <c r="E7" s="98" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="95"/>
+      <c r="F7" s="99"/>
       <c r="G7" s="33" t="s">
         <v>25</v>
       </c>
@@ -2649,14 +2651,14 @@
       <c r="K7" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="L7" s="95" t="s">
+      <c r="L7" s="99" t="s">
         <v>27</v>
       </c>
-      <c r="M7" s="96"/>
-      <c r="N7" s="97" t="s">
+      <c r="M7" s="100"/>
+      <c r="N7" s="101" t="s">
         <v>28</v>
       </c>
-      <c r="O7" s="98"/>
+      <c r="O7" s="102"/>
       <c r="P7" s="36"/>
       <c r="Q7" s="36"/>
       <c r="R7" s="36"/>
@@ -2664,15 +2666,15 @@
     <row r="8" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E8" s="16">
         <f>ATAN2(M4, N4)</f>
-        <v>-0.96406927039984291</v>
+        <v>-0.37566451469282719</v>
       </c>
       <c r="F8" s="29">
         <f>DEGREES(E8)</f>
-        <v>-55.237100352167545</v>
+        <v>-21.523991204729302</v>
       </c>
       <c r="G8" s="29">
         <f>SQRT(M4*M4+N4*N4)</f>
-        <v>103.46692249560083</v>
+        <v>109.02427023839802</v>
       </c>
       <c r="H8" s="47" t="str">
         <f>IF(C6 + C7 &gt;G8, "TRUE", "FALSE")</f>
@@ -2680,7 +2682,7 @@
       </c>
       <c r="I8" s="17">
         <f>C6*C6</f>
-        <v>7225</v>
+        <v>7056</v>
       </c>
       <c r="J8" s="17">
         <f>C7*C7</f>
@@ -2688,23 +2690,23 @@
       </c>
       <c r="K8" s="35">
         <f>G8*G8</f>
-        <v>10705.404050710669</v>
+        <v>11886.291501015239</v>
       </c>
       <c r="L8" s="29">
         <f>ACOS((I8 + K8 - J8) / (2 * C6 * G8))</f>
-        <v>1.6819211450481926</v>
+        <v>1.6220693096897711</v>
       </c>
       <c r="M8" s="29">
         <f>DEGREES(L8)</f>
-        <v>96.366983085072192</v>
+        <v>92.937725522922776</v>
       </c>
       <c r="N8" s="14">
         <f>ACOS(( J8 + I8 - K8) / (2 * C7 * C6))</f>
-        <v>0.81727172679455284</v>
+        <v>0.88230526008940935</v>
       </c>
       <c r="O8" s="30">
         <f>DEGREES(N8)</f>
-        <v>46.826220660696755</v>
+        <v>50.552367645315549</v>
       </c>
       <c r="P8" s="37"/>
       <c r="Q8" s="37"/>
@@ -2715,7 +2717,7 @@
         <v>0</v>
       </c>
       <c r="C9" s="8">
-        <v>70</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.25">
@@ -2723,7 +2725,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="10">
-        <v>-85</v>
+        <v>-40</v>
       </c>
     </row>
     <row r="11" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2731,7 +2733,7 @@
         <v>2</v>
       </c>
       <c r="C11" s="12">
-        <v>70</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -2750,7 +2752,7 @@
       </c>
       <c r="C14" s="31">
         <f>C3 - M8 - F8</f>
-        <v>93.870117267095353</v>
+        <v>29.586265681806527</v>
       </c>
     </row>
     <row r="15" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2759,7 +2761,7 @@
       </c>
       <c r="C15" s="32">
         <f>O8-C4</f>
-        <v>1.8262206606967553</v>
+        <v>3.5523676453155488</v>
       </c>
     </row>
   </sheetData>
@@ -3368,11 +3370,11 @@
         <v>0</v>
       </c>
       <c r="C3" s="78">
-        <f>B3 * ($J$12 - $J$11) / 180 + $J$11</f>
+        <f t="shared" ref="C3:C39" si="0">B3 * ($J$12 - $J$11) / 180 + $J$11</f>
         <v>45</v>
       </c>
       <c r="D3" s="70">
-        <f>$I$10*SIN(RADIANS(C3))</f>
+        <f t="shared" ref="D3:D39" si="1">$I$10*SIN(RADIANS(C3))</f>
         <v>5.7999999999999989</v>
       </c>
       <c r="E3" s="70">
@@ -3380,7 +3382,7 @@
         <v>5.8</v>
       </c>
       <c r="F3" s="86">
-        <f>$I$10*COS(RADIANS(C3))</f>
+        <f t="shared" ref="F3:F39" si="2">$I$10*COS(RADIANS(C3))</f>
         <v>5.8</v>
       </c>
       <c r="H3" s="83" t="s">
@@ -3395,19 +3397,19 @@
         <v>5</v>
       </c>
       <c r="C4" s="78">
-        <f>B4 * ($J$12 - $J$11) / 180 + $J$11</f>
+        <f t="shared" si="0"/>
         <v>47.5</v>
       </c>
       <c r="D4" s="70">
-        <f>$I$10*SIN(RADIANS(C4))</f>
+        <f t="shared" si="1"/>
         <v>6.0474721318937243</v>
       </c>
       <c r="E4" s="70">
-        <f t="shared" ref="E4:E39" si="0">B4 * ($I$8 - $I$4) / 180 + $I$4</f>
+        <f t="shared" ref="E4:E39" si="3">B4 * ($I$8 - $I$4) / 180 + $I$4</f>
         <v>5.4777777777777779</v>
       </c>
       <c r="F4" s="86">
-        <f>$I$10*COS(RADIANS(C4))</f>
+        <f t="shared" si="2"/>
         <v>5.5414872384558258</v>
       </c>
       <c r="H4" s="57" t="s">
@@ -3422,19 +3424,19 @@
         <v>10</v>
       </c>
       <c r="C5" s="78">
-        <f>B5 * ($J$12 - $J$11) / 180 + $J$11</f>
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
       <c r="D5" s="70">
-        <f>$I$10*SIN(RADIANS(C5))</f>
+        <f t="shared" si="1"/>
         <v>6.283432556868541</v>
       </c>
       <c r="E5" s="70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5.155555555555555</v>
       </c>
       <c r="F5" s="86">
-        <f>$I$10*COS(RADIANS(C5))</f>
+        <f t="shared" si="2"/>
         <v>5.2724259409957073</v>
       </c>
     </row>
@@ -3443,19 +3445,19 @@
         <v>15</v>
       </c>
       <c r="C6" s="78">
-        <f>B6 * ($J$12 - $J$11) / 180 + $J$11</f>
+        <f t="shared" si="0"/>
         <v>52.5</v>
       </c>
       <c r="D6" s="70">
-        <f>$I$10*SIN(RADIANS(C6))</f>
+        <f t="shared" si="1"/>
         <v>6.5074321108443991</v>
       </c>
       <c r="E6" s="70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>4.833333333333333</v>
       </c>
       <c r="F6" s="86">
-        <f>$I$10*COS(RADIANS(C6))</f>
+        <f t="shared" si="2"/>
         <v>4.9933282810918014</v>
       </c>
       <c r="H6" s="55" t="s">
@@ -3470,19 +3472,19 @@
         <v>20</v>
       </c>
       <c r="C7" s="78">
-        <f>B7 * ($J$12 - $J$11) / 180 + $J$11</f>
+        <f t="shared" si="0"/>
         <v>55</v>
       </c>
       <c r="D7" s="70">
-        <f>$I$10*SIN(RADIANS(C7))</f>
+        <f t="shared" si="1"/>
         <v>6.7190443979390029</v>
       </c>
       <c r="E7" s="70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>4.5111111111111111</v>
       </c>
       <c r="F7" s="86">
-        <f>$I$10*COS(RADIANS(C7))</f>
+        <f t="shared" si="2"/>
         <v>4.7047255370026111</v>
       </c>
       <c r="H7" s="83" t="s">
@@ -3497,19 +3499,19 @@
         <v>25</v>
       </c>
       <c r="C8" s="78">
-        <f>B8 * ($J$12 - $J$11) / 180 + $J$11</f>
+        <f t="shared" si="0"/>
         <v>57.5</v>
       </c>
       <c r="D8" s="70">
-        <f>$I$10*SIN(RADIANS(C8))</f>
+        <f t="shared" si="1"/>
         <v>6.91786660213661</v>
       </c>
       <c r="E8" s="70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>4.1888888888888882</v>
       </c>
       <c r="F8" s="86">
-        <f>$I$10*COS(RADIANS(C8))</f>
+        <f t="shared" si="2"/>
         <v>4.4071670804546175</v>
       </c>
       <c r="H8" s="57" t="s">
@@ -3524,19 +3526,19 @@
         <v>30</v>
       </c>
       <c r="C9" s="78">
-        <f>B9 * ($J$12 - $J$11) / 180 + $J$11</f>
+        <f t="shared" si="0"/>
         <v>60</v>
       </c>
       <c r="D9" s="70">
-        <f>$I$10*SIN(RADIANS(C9))</f>
+        <f t="shared" si="1"/>
         <v>7.1035202540712161</v>
       </c>
       <c r="E9" s="70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>3.8666666666666663</v>
       </c>
       <c r="F9" s="86">
-        <f>$I$10*COS(RADIANS(C9))</f>
+        <f t="shared" si="2"/>
         <v>4.1012193308819764</v>
       </c>
     </row>
@@ -3545,48 +3547,48 @@
         <v>35</v>
       </c>
       <c r="C10" s="78">
-        <f>B10 * ($J$12 - $J$11) / 180 + $J$11</f>
+        <f t="shared" si="0"/>
         <v>62.5</v>
       </c>
       <c r="D10" s="70">
-        <f>$I$10*SIN(RADIANS(C10))</f>
+        <f t="shared" si="1"/>
         <v>7.2756519514644999</v>
       </c>
       <c r="E10" s="70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>3.5444444444444443</v>
       </c>
       <c r="F10" s="86">
-        <f>$I$10*COS(RADIANS(C10))</f>
+        <f t="shared" si="2"/>
         <v>3.7874646772149312</v>
       </c>
       <c r="H10" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="I10" s="100">
+      <c r="I10" s="104">
         <f>SQRT((I4)^2 + (I2)^2)</f>
         <v>8.2024386617639511</v>
       </c>
-      <c r="J10" s="101"/>
+      <c r="J10" s="105"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="76">
         <v>40</v>
       </c>
       <c r="C11" s="78">
-        <f>B11 * ($J$12 - $J$11) / 180 + $J$11</f>
+        <f t="shared" si="0"/>
         <v>65</v>
       </c>
       <c r="D11" s="70">
-        <f>$I$10*SIN(RADIANS(C11))</f>
+        <f t="shared" si="1"/>
         <v>7.433934031847147</v>
       </c>
       <c r="E11" s="70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>3.2222222222222219</v>
       </c>
       <c r="F11" s="86">
-        <f>$I$10*COS(RADIANS(C11))</f>
+        <f t="shared" si="2"/>
         <v>3.4665003692693901</v>
       </c>
       <c r="H11" s="79" t="s">
@@ -3606,19 +3608,19 @@
         <v>45</v>
       </c>
       <c r="C12" s="78">
-        <f>B12 * ($J$12 - $J$11) / 180 + $J$11</f>
+        <f t="shared" si="0"/>
         <v>67.5</v>
       </c>
       <c r="D12" s="70">
-        <f>$I$10*SIN(RADIANS(C12))</f>
+        <f t="shared" si="1"/>
         <v>7.5780651962829833</v>
       </c>
       <c r="E12" s="70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>2.9</v>
       </c>
       <c r="F12" s="86">
-        <f>$I$10*COS(RADIANS(C12))</f>
+        <f t="shared" si="2"/>
         <v>3.1389373808479428</v>
       </c>
       <c r="H12" s="54" t="s">
@@ -3638,19 +3640,19 @@
         <v>50</v>
       </c>
       <c r="C13" s="78">
-        <f>B13 * ($J$12 - $J$11) / 180 + $J$11</f>
+        <f t="shared" si="0"/>
         <v>70</v>
       </c>
       <c r="D13" s="70">
-        <f>$I$10*SIN(RADIANS(C13))</f>
+        <f t="shared" si="1"/>
         <v>7.7077710829086259</v>
       </c>
       <c r="E13" s="70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>2.5777777777777775</v>
       </c>
       <c r="F13" s="86">
-        <f>$I$10*COS(RADIANS(C13))</f>
+        <f t="shared" si="2"/>
         <v>2.8053992467165139</v>
       </c>
     </row>
@@ -3659,19 +3661,19 @@
         <v>55</v>
       </c>
       <c r="C14" s="78">
-        <f>B14 * ($J$12 - $J$11) / 180 + $J$11</f>
+        <f t="shared" si="0"/>
         <v>72.5</v>
       </c>
       <c r="D14" s="70">
-        <f>$I$10*SIN(RADIANS(C14))</f>
+        <f t="shared" si="1"/>
         <v>7.8228047891968826</v>
       </c>
       <c r="E14" s="70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>2.2555555555555555</v>
       </c>
       <c r="F14" s="86">
-        <f>$I$10*COS(RADIANS(C14))</f>
+        <f t="shared" si="2"/>
         <v>2.4665208756704886</v>
       </c>
     </row>
@@ -3680,19 +3682,19 @@
         <v>60</v>
       </c>
       <c r="C15" s="78">
-        <f>B15 * ($J$12 - $J$11) / 180 + $J$11</f>
+        <f t="shared" si="0"/>
         <v>75</v>
       </c>
       <c r="D15" s="70">
-        <f>$I$10*SIN(RADIANS(C15))</f>
+        <f t="shared" si="1"/>
         <v>7.9229473419497438</v>
       </c>
       <c r="E15" s="70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1.9333333333333331</v>
       </c>
       <c r="F15" s="86">
-        <f>$I$10*COS(RADIANS(C15))</f>
+        <f t="shared" si="2"/>
         <v>2.122947341949744</v>
       </c>
     </row>
@@ -3701,19 +3703,19 @@
         <v>65</v>
       </c>
       <c r="C16" s="78">
-        <f>B16 * ($J$12 - $J$11) / 180 + $J$11</f>
+        <f t="shared" si="0"/>
         <v>77.5</v>
       </c>
       <c r="D16" s="70">
-        <f>$I$10*SIN(RADIANS(C16))</f>
+        <f t="shared" si="1"/>
         <v>8.0080081141263157</v>
       </c>
       <c r="E16" s="70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1.6111111111111107</v>
       </c>
       <c r="F16" s="86">
-        <f>$I$10*COS(RADIANS(C16))</f>
+        <f t="shared" si="2"/>
         <v>1.7753326573031589</v>
       </c>
     </row>
@@ -3722,19 +3724,19 @@
         <v>70</v>
       </c>
       <c r="C17" s="78">
-        <f>B17 * ($J$12 - $J$11) / 180 + $J$11</f>
+        <f t="shared" si="0"/>
         <v>80</v>
       </c>
       <c r="D17" s="70">
-        <f>$I$10*SIN(RADIANS(C17))</f>
+        <f t="shared" si="1"/>
         <v>8.0778251877122198</v>
       </c>
       <c r="E17" s="70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1.2888888888888888</v>
       </c>
       <c r="F17" s="86">
-        <f>$I$10*COS(RADIANS(C17))</f>
+        <f t="shared" si="2"/>
         <v>1.4243385260400856</v>
       </c>
     </row>
@@ -3743,19 +3745,19 @@
         <v>75</v>
       </c>
       <c r="C18" s="78">
-        <f>B18 * ($J$12 - $J$11) / 180 + $J$11</f>
+        <f t="shared" si="0"/>
         <v>82.5</v>
       </c>
       <c r="D18" s="70">
-        <f>$I$10*SIN(RADIANS(C18))</f>
+        <f t="shared" si="1"/>
         <v>8.1322656619397424</v>
       </c>
       <c r="E18" s="70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.96666666666666679</v>
       </c>
       <c r="F18" s="86">
-        <f>$I$10*COS(RADIANS(C18))</f>
+        <f t="shared" si="2"/>
         <v>1.0706330854385853</v>
       </c>
     </row>
@@ -3764,19 +3766,19 @@
         <v>80</v>
       </c>
       <c r="C19" s="78">
-        <f>B19 * ($J$12 - $J$11) / 180 + $J$11</f>
+        <f t="shared" si="0"/>
         <v>85</v>
       </c>
       <c r="D19" s="70">
-        <f>$I$10*SIN(RADIANS(C19))</f>
+        <f t="shared" si="1"/>
         <v>8.1712259062720012</v>
       </c>
       <c r="E19" s="70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.64444444444444393</v>
       </c>
       <c r="F19" s="86">
-        <f>$I$10*COS(RADIANS(C19))</f>
+        <f t="shared" si="2"/>
         <v>0.7148896339081442</v>
       </c>
     </row>
@@ -3785,19 +3787,19 @@
         <v>85</v>
       </c>
       <c r="C20" s="78">
-        <f>B20 * ($J$12 - $J$11) / 180 + $J$11</f>
+        <f t="shared" si="0"/>
         <v>87.5</v>
       </c>
       <c r="D20" s="70">
-        <f>$I$10*SIN(RADIANS(C20))</f>
+        <f t="shared" si="1"/>
         <v>8.1946317576695495</v>
       </c>
       <c r="E20" s="70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.32222222222222197</v>
       </c>
       <c r="F20" s="86">
-        <f>$I$10*COS(RADIANS(C20))</f>
+        <f t="shared" si="2"/>
         <v>0.35778534932789008</v>
       </c>
     </row>
@@ -3806,19 +3808,19 @@
         <v>90</v>
       </c>
       <c r="C21" s="78">
-        <f>B21 * ($J$12 - $J$11) / 180 + $J$11</f>
+        <f t="shared" si="0"/>
         <v>90</v>
       </c>
       <c r="D21" s="70">
-        <f>$I$10*SIN(RADIANS(C21))</f>
+        <f t="shared" si="1"/>
         <v>8.2024386617639511</v>
       </c>
       <c r="E21" s="70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F21" s="86">
-        <f>$I$10*COS(RADIANS(C21))</f>
+        <f t="shared" si="2"/>
         <v>5.0246025264714163E-16</v>
       </c>
     </row>
@@ -3827,19 +3829,19 @@
         <v>95</v>
       </c>
       <c r="C22" s="78">
-        <f>B22 * ($J$12 - $J$11) / 180 + $J$11</f>
+        <f t="shared" si="0"/>
         <v>92.5</v>
       </c>
       <c r="D22" s="70">
-        <f>$I$10*SIN(RADIANS(C22))</f>
+        <f t="shared" si="1"/>
         <v>8.1946317576695495</v>
       </c>
       <c r="E22" s="70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-0.32222222222222197</v>
       </c>
       <c r="F22" s="86">
-        <f>$I$10*COS(RADIANS(C22))</f>
+        <f t="shared" si="2"/>
         <v>-0.35778534932788908</v>
       </c>
     </row>
@@ -3848,19 +3850,19 @@
         <v>100</v>
       </c>
       <c r="C23" s="78">
-        <f>B23 * ($J$12 - $J$11) / 180 + $J$11</f>
+        <f t="shared" si="0"/>
         <v>95</v>
       </c>
       <c r="D23" s="70">
-        <f>$I$10*SIN(RADIANS(C23))</f>
+        <f t="shared" si="1"/>
         <v>8.1712259062720012</v>
       </c>
       <c r="E23" s="70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-0.64444444444444482</v>
       </c>
       <c r="F23" s="86">
-        <f>$I$10*COS(RADIANS(C23))</f>
+        <f t="shared" si="2"/>
         <v>-0.71488963390814497</v>
       </c>
     </row>
@@ -3869,19 +3871,19 @@
         <v>105</v>
       </c>
       <c r="C24" s="78">
-        <f>B24 * ($J$12 - $J$11) / 180 + $J$11</f>
+        <f t="shared" si="0"/>
         <v>97.5</v>
       </c>
       <c r="D24" s="70">
-        <f>$I$10*SIN(RADIANS(C24))</f>
+        <f t="shared" si="1"/>
         <v>8.1322656619397424</v>
       </c>
       <c r="E24" s="70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-0.96666666666666679</v>
       </c>
       <c r="F24" s="86">
-        <f>$I$10*COS(RADIANS(C24))</f>
+        <f t="shared" si="2"/>
         <v>-1.0706330854385844</v>
       </c>
       <c r="H24" s="68"/>
@@ -3891,19 +3893,19 @@
         <v>110</v>
       </c>
       <c r="C25" s="78">
-        <f>B25 * ($J$12 - $J$11) / 180 + $J$11</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="D25" s="70">
-        <f>$I$10*SIN(RADIANS(C25))</f>
+        <f t="shared" si="1"/>
         <v>8.0778251877122198</v>
       </c>
       <c r="E25" s="70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-1.2888888888888888</v>
       </c>
       <c r="F25" s="86">
-        <f>$I$10*COS(RADIANS(C25))</f>
+        <f t="shared" si="2"/>
         <v>-1.4243385260400847</v>
       </c>
     </row>
@@ -3912,19 +3914,19 @@
         <v>115</v>
       </c>
       <c r="C26" s="78">
-        <f>B26 * ($J$12 - $J$11) / 180 + $J$11</f>
+        <f t="shared" si="0"/>
         <v>102.5</v>
       </c>
       <c r="D26" s="70">
-        <f>$I$10*SIN(RADIANS(C26))</f>
+        <f t="shared" si="1"/>
         <v>8.0080081141263157</v>
       </c>
       <c r="E26" s="70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-1.6111111111111116</v>
       </c>
       <c r="F26" s="86">
-        <f>$I$10*COS(RADIANS(C26))</f>
+        <f t="shared" si="2"/>
         <v>-1.775332657303158</v>
       </c>
     </row>
@@ -3933,19 +3935,19 @@
         <v>120</v>
       </c>
       <c r="C27" s="78">
-        <f>B27 * ($J$12 - $J$11) / 180 + $J$11</f>
+        <f t="shared" si="0"/>
         <v>105</v>
       </c>
       <c r="D27" s="70">
-        <f>$I$10*SIN(RADIANS(C27))</f>
+        <f t="shared" si="1"/>
         <v>7.9229473419497438</v>
       </c>
       <c r="E27" s="70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-1.9333333333333336</v>
       </c>
       <c r="F27" s="86">
-        <f>$I$10*COS(RADIANS(C27))</f>
+        <f t="shared" si="2"/>
         <v>-2.1229473419497449</v>
       </c>
     </row>
@@ -3954,19 +3956,19 @@
         <v>125</v>
       </c>
       <c r="C28" s="78">
-        <f>B28 * ($J$12 - $J$11) / 180 + $J$11</f>
+        <f t="shared" si="0"/>
         <v>107.5</v>
       </c>
       <c r="D28" s="70">
-        <f>$I$10*SIN(RADIANS(C28))</f>
+        <f t="shared" si="1"/>
         <v>7.8228047891968826</v>
       </c>
       <c r="E28" s="70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-2.2555555555555555</v>
       </c>
       <c r="F28" s="86">
-        <f>$I$10*COS(RADIANS(C28))</f>
+        <f t="shared" si="2"/>
         <v>-2.4665208756704891</v>
       </c>
     </row>
@@ -3975,19 +3977,19 @@
         <v>130</v>
       </c>
       <c r="C29" s="78">
-        <f>B29 * ($J$12 - $J$11) / 180 + $J$11</f>
+        <f t="shared" si="0"/>
         <v>110</v>
       </c>
       <c r="D29" s="70">
-        <f>$I$10*SIN(RADIANS(C29))</f>
+        <f t="shared" si="1"/>
         <v>7.7077710829086268</v>
       </c>
       <c r="E29" s="70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-2.5777777777777784</v>
       </c>
       <c r="F29" s="86">
-        <f>$I$10*COS(RADIANS(C29))</f>
+        <f t="shared" si="2"/>
         <v>-2.805399246716513</v>
       </c>
     </row>
@@ -3996,19 +3998,19 @@
         <v>135</v>
       </c>
       <c r="C30" s="78">
-        <f>B30 * ($J$12 - $J$11) / 180 + $J$11</f>
+        <f t="shared" si="0"/>
         <v>112.5</v>
       </c>
       <c r="D30" s="70">
-        <f>$I$10*SIN(RADIANS(C30))</f>
+        <f t="shared" si="1"/>
         <v>7.5780651962829833</v>
       </c>
       <c r="E30" s="70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-2.8999999999999995</v>
       </c>
       <c r="F30" s="86">
-        <f>$I$10*COS(RADIANS(C30))</f>
+        <f t="shared" si="2"/>
         <v>-3.1389373808479419</v>
       </c>
     </row>
@@ -4017,19 +4019,19 @@
         <v>140</v>
       </c>
       <c r="C31" s="78">
-        <f>B31 * ($J$12 - $J$11) / 180 + $J$11</f>
+        <f t="shared" si="0"/>
         <v>115</v>
       </c>
       <c r="D31" s="70">
-        <f>$I$10*SIN(RADIANS(C31))</f>
+        <f t="shared" si="1"/>
         <v>7.4339340318471478</v>
       </c>
       <c r="E31" s="70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-3.2222222222222223</v>
       </c>
       <c r="F31" s="86">
-        <f>$I$10*COS(RADIANS(C31))</f>
+        <f t="shared" si="2"/>
         <v>-3.4665003692693892</v>
       </c>
     </row>
@@ -4038,19 +4040,19 @@
         <v>145</v>
       </c>
       <c r="C32" s="78">
-        <f>B32 * ($J$12 - $J$11) / 180 + $J$11</f>
+        <f t="shared" si="0"/>
         <v>117.5</v>
       </c>
       <c r="D32" s="70">
-        <f>$I$10*SIN(RADIANS(C32))</f>
+        <f t="shared" si="1"/>
         <v>7.2756519514645008</v>
       </c>
       <c r="E32" s="70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-3.5444444444444452</v>
       </c>
       <c r="F32" s="86">
-        <f>$I$10*COS(RADIANS(C32))</f>
+        <f t="shared" si="2"/>
         <v>-3.7874646772149303</v>
       </c>
     </row>
@@ -4059,19 +4061,19 @@
         <v>150</v>
       </c>
       <c r="C33" s="78">
-        <f>B33 * ($J$12 - $J$11) / 180 + $J$11</f>
+        <f t="shared" si="0"/>
         <v>120</v>
       </c>
       <c r="D33" s="70">
-        <f>$I$10*SIN(RADIANS(C33))</f>
+        <f t="shared" si="1"/>
         <v>7.103520254071217</v>
       </c>
       <c r="E33" s="70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-3.8666666666666663</v>
       </c>
       <c r="F33" s="86">
-        <f>$I$10*COS(RADIANS(C33))</f>
+        <f t="shared" si="2"/>
         <v>-4.1012193308819738</v>
       </c>
     </row>
@@ -4080,19 +4082,19 @@
         <v>155</v>
       </c>
       <c r="C34" s="78">
-        <f>B34 * ($J$12 - $J$11) / 180 + $J$11</f>
+        <f t="shared" si="0"/>
         <v>122.5</v>
       </c>
       <c r="D34" s="70">
-        <f>$I$10*SIN(RADIANS(C34))</f>
+        <f t="shared" si="1"/>
         <v>6.9178666021366091</v>
       </c>
       <c r="E34" s="70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-4.1888888888888891</v>
       </c>
       <c r="F34" s="86">
-        <f>$I$10*COS(RADIANS(C34))</f>
+        <f t="shared" si="2"/>
         <v>-4.4071670804546184</v>
       </c>
     </row>
@@ -4101,19 +4103,19 @@
         <v>160</v>
       </c>
       <c r="C35" s="78">
-        <f>B35 * ($J$12 - $J$11) / 180 + $J$11</f>
+        <f t="shared" si="0"/>
         <v>125</v>
       </c>
       <c r="D35" s="70">
-        <f>$I$10*SIN(RADIANS(C35))</f>
+        <f t="shared" si="1"/>
         <v>6.719044397939002</v>
       </c>
       <c r="E35" s="70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-4.511111111111112</v>
       </c>
       <c r="F35" s="86">
-        <f>$I$10*COS(RADIANS(C35))</f>
+        <f t="shared" si="2"/>
         <v>-4.7047255370026111</v>
       </c>
     </row>
@@ -4122,19 +4124,19 @@
         <v>165</v>
       </c>
       <c r="C36" s="78">
-        <f>B36 * ($J$12 - $J$11) / 180 + $J$11</f>
+        <f t="shared" si="0"/>
         <v>127.5</v>
       </c>
       <c r="D36" s="70">
-        <f>$I$10*SIN(RADIANS(C36))</f>
+        <f t="shared" si="1"/>
         <v>6.5074321108443991</v>
       </c>
       <c r="E36" s="70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-4.833333333333333</v>
       </c>
       <c r="F36" s="86">
-        <f>$I$10*COS(RADIANS(C36))</f>
+        <f t="shared" si="2"/>
         <v>-4.9933282810918014</v>
       </c>
     </row>
@@ -4143,19 +4145,19 @@
         <v>170</v>
       </c>
       <c r="C37" s="78">
-        <f>B37 * ($J$12 - $J$11) / 180 + $J$11</f>
+        <f t="shared" si="0"/>
         <v>130</v>
       </c>
       <c r="D37" s="70">
-        <f>$I$10*SIN(RADIANS(C37))</f>
+        <f t="shared" si="1"/>
         <v>6.283432556868541</v>
       </c>
       <c r="E37" s="70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-5.1555555555555559</v>
       </c>
       <c r="F37" s="86">
-        <f>$I$10*COS(RADIANS(C37))</f>
+        <f t="shared" si="2"/>
         <v>-5.2724259409957073</v>
       </c>
     </row>
@@ -4164,19 +4166,19 @@
         <v>175</v>
       </c>
       <c r="C38" s="78">
-        <f>B38 * ($J$12 - $J$11) / 180 + $J$11</f>
+        <f t="shared" si="0"/>
         <v>132.5</v>
       </c>
       <c r="D38" s="70">
-        <f>$I$10*SIN(RADIANS(C38))</f>
+        <f t="shared" si="1"/>
         <v>6.0474721318937243</v>
       </c>
       <c r="E38" s="70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-5.4777777777777787</v>
       </c>
       <c r="F38" s="86">
-        <f>$I$10*COS(RADIANS(C38))</f>
+        <f t="shared" si="2"/>
         <v>-5.5414872384558258</v>
       </c>
     </row>
@@ -4185,19 +4187,19 @@
         <v>180</v>
       </c>
       <c r="C39" s="78">
-        <f>B39 * ($J$12 - $J$11) / 180 + $J$11</f>
+        <f t="shared" si="0"/>
         <v>135</v>
       </c>
       <c r="D39" s="70">
-        <f>$I$10*SIN(RADIANS(C39))</f>
+        <f t="shared" si="1"/>
         <v>5.8</v>
       </c>
       <c r="E39" s="70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-5.8</v>
       </c>
       <c r="F39" s="86">
-        <f>$I$10*COS(RADIANS(C39))</f>
+        <f t="shared" si="2"/>
         <v>-5.7999999999999989</v>
       </c>
     </row>
@@ -4975,15 +4977,15 @@
         <v>0</v>
       </c>
       <c r="C3" s="70">
-        <f>$H$11*SIN(RADIANS(180 - B3)) + $H$2</f>
+        <f t="shared" ref="C3:C39" si="0">$H$11*SIN(RADIANS(180 - B3)) + $H$2</f>
         <v>4.0000000000000009</v>
       </c>
       <c r="D3" s="70">
-        <f>$H$12 * SIN(RADIANS(B3)) + $H$3</f>
+        <f t="shared" ref="D3:D39" si="1">$H$12 * SIN(RADIANS(B3)) + $H$3</f>
         <v>0</v>
       </c>
       <c r="E3" s="86">
-        <f>$H$10*COS(RADIANS(180 - B3)) + $H$4 + $H$10</f>
+        <f t="shared" ref="E3:E39" si="2">$H$10*COS(RADIANS(180 - B3)) + $H$4 + $H$10</f>
         <v>8</v>
       </c>
       <c r="G3" s="83" t="s">
@@ -4998,15 +5000,15 @@
         <v>5</v>
       </c>
       <c r="C4" s="70">
-        <f>$H$11*SIN(RADIANS(180 - B4)) + $H$2</f>
+        <f t="shared" si="0"/>
         <v>4.3486229709906326</v>
       </c>
       <c r="D4" s="70">
-        <f>$H$12 * SIN(RADIANS(B4)) + $H$3</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E4" s="86">
-        <f>$H$10*COS(RADIANS(180 - B4)) + $H$4 + $H$10</f>
+        <f t="shared" si="2"/>
         <v>7.9737434168330434</v>
       </c>
       <c r="G4" s="57" t="s">
@@ -5021,15 +5023,15 @@
         <v>10</v>
       </c>
       <c r="C5" s="70">
-        <f>$H$11*SIN(RADIANS(180 - B5)) + $H$2</f>
+        <f t="shared" si="0"/>
         <v>4.6945927106677212</v>
       </c>
       <c r="D5" s="70">
-        <f>$H$12 * SIN(RADIANS(B5)) + $H$3</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E5" s="86">
-        <f>$H$10*COS(RADIANS(180 - B5)) + $H$4 + $H$10</f>
+        <f t="shared" si="2"/>
         <v>7.8951734957842366</v>
       </c>
     </row>
@@ -5038,15 +5040,15 @@
         <v>15</v>
       </c>
       <c r="C6" s="70">
-        <f>$H$11*SIN(RADIANS(180 - B6)) + $H$2</f>
+        <f t="shared" si="0"/>
         <v>5.0352761804100838</v>
       </c>
       <c r="D6" s="70">
-        <f>$H$12 * SIN(RADIANS(B6)) + $H$3</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E6" s="86">
-        <f>$H$10*COS(RADIANS(180 - B6)) + $H$4 + $H$10</f>
+        <f t="shared" si="2"/>
         <v>7.7648882013945713</v>
       </c>
       <c r="G6" s="55" t="s">
@@ -5061,15 +5063,15 @@
         <v>20</v>
       </c>
       <c r="C7" s="70">
-        <f>$H$11*SIN(RADIANS(180 - B7)) + $H$2</f>
+        <f t="shared" si="0"/>
         <v>5.3680805733026755</v>
       </c>
       <c r="D7" s="70">
-        <f>$H$12 * SIN(RADIANS(B7)) + $H$3</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E7" s="86">
-        <f>$H$10*COS(RADIANS(180 - B7)) + $H$4 + $H$10</f>
+        <f t="shared" si="2"/>
         <v>7.583879083422767</v>
       </c>
       <c r="G7" s="83" t="s">
@@ -5084,15 +5086,15 @@
         <v>25</v>
       </c>
       <c r="C8" s="70">
-        <f>$H$11*SIN(RADIANS(180 - B8)) + $H$2</f>
+        <f t="shared" si="0"/>
         <v>5.690473046962798</v>
       </c>
       <c r="D8" s="70">
-        <f>$H$12 * SIN(RADIANS(B8)) + $H$3</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E8" s="86">
-        <f>$H$10*COS(RADIANS(180 - B8)) + $H$4 + $H$10</f>
+        <f t="shared" si="2"/>
         <v>7.3535237305528849</v>
       </c>
       <c r="G8" s="57" t="s">
@@ -5107,15 +5109,15 @@
         <v>30</v>
       </c>
       <c r="C9" s="70">
-        <f>$H$11*SIN(RADIANS(180 - B9)) + $H$2</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="D9" s="70">
-        <f>$H$12 * SIN(RADIANS(B9)) + $H$3</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E9" s="86">
-        <f>$H$10*COS(RADIANS(180 - B9)) + $H$4 + $H$10</f>
+        <f t="shared" si="2"/>
         <v>7.0755752861126258</v>
       </c>
     </row>
@@ -5124,21 +5126,21 @@
         <v>35</v>
       </c>
       <c r="C10" s="70">
-        <f>$H$11*SIN(RADIANS(180 - B10)) + $H$2</f>
+        <f t="shared" si="0"/>
         <v>6.2943057454041842</v>
       </c>
       <c r="D10" s="70">
-        <f>$H$12 * SIN(RADIANS(B10)) + $H$3</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E10" s="86">
-        <f>$H$10*COS(RADIANS(180 - B10)) + $H$4 + $H$10</f>
+        <f t="shared" si="2"/>
         <v>6.7521491055940448</v>
       </c>
       <c r="G10" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="H10" s="102">
+      <c r="H10" s="87">
         <f>(H8-H4) / 2</f>
         <v>-6.9</v>
       </c>
@@ -5148,21 +5150,21 @@
         <v>40</v>
       </c>
       <c r="C11" s="70">
-        <f>$H$11*SIN(RADIANS(180 - B11)) + $H$2</f>
+        <f t="shared" si="0"/>
         <v>6.5711504387461579</v>
       </c>
       <c r="D11" s="70">
-        <f>$H$12 * SIN(RADIANS(B11)) + $H$3</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E11" s="86">
-        <f>$H$10*COS(RADIANS(180 - B11)) + $H$4 + $H$10</f>
+        <f t="shared" si="2"/>
         <v>6.3857066575209469</v>
       </c>
       <c r="G11" s="79" t="s">
         <v>47</v>
       </c>
-      <c r="H11" s="103">
+      <c r="H11" s="88">
         <f>(H6-H2)</f>
         <v>4</v>
       </c>
@@ -5172,21 +5174,21 @@
         <v>45</v>
       </c>
       <c r="C12" s="70">
-        <f>$H$11*SIN(RADIANS(180 - B12)) + $H$2</f>
+        <f t="shared" si="0"/>
         <v>6.8284271247461898</v>
       </c>
       <c r="D12" s="70">
-        <f>$H$12 * SIN(RADIANS(B12)) + $H$3</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E12" s="86">
-        <f>$H$10*COS(RADIANS(180 - B12)) + $H$4 + $H$10</f>
+        <f t="shared" si="2"/>
         <v>5.9790367901871786</v>
       </c>
       <c r="G12" s="54" t="s">
         <v>48</v>
       </c>
-      <c r="H12" s="104">
+      <c r="H12" s="89">
         <f>(H7-H3)</f>
         <v>0</v>
       </c>
@@ -5196,69 +5198,69 @@
         <v>50</v>
       </c>
       <c r="C13" s="70">
-        <f>$H$11*SIN(RADIANS(180 - B13)) + $H$2</f>
+        <f t="shared" si="0"/>
         <v>7.0641777724759116</v>
       </c>
       <c r="D13" s="70">
-        <f>$H$12 * SIN(RADIANS(B13)) + $H$3</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E13" s="86">
-        <f>$H$10*COS(RADIANS(180 - B13)) + $H$4 + $H$10</f>
+        <f t="shared" si="2"/>
         <v>5.5352345068371225</v>
       </c>
-      <c r="I13" s="105"/>
+      <c r="I13" s="90"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="76">
         <v>55</v>
       </c>
       <c r="C14" s="70">
-        <f>$H$11*SIN(RADIANS(180 - B14)) + $H$2</f>
+        <f t="shared" si="0"/>
         <v>7.2766081771559668</v>
       </c>
       <c r="D14" s="70">
-        <f>$H$12 * SIN(RADIANS(B14)) + $H$3</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E14" s="86">
-        <f>$H$10*COS(RADIANS(180 - B14)) + $H$4 + $H$10</f>
+        <f t="shared" si="2"/>
         <v>5.0576774108222189</v>
       </c>
-      <c r="I14" s="105"/>
+      <c r="I14" s="90"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="76">
         <v>60</v>
       </c>
       <c r="C15" s="70">
-        <f>$H$11*SIN(RADIANS(180 - B15)) + $H$2</f>
+        <f t="shared" si="0"/>
         <v>7.4641016151377553</v>
       </c>
       <c r="D15" s="70">
-        <f>$H$12 * SIN(RADIANS(B15)) + $H$3</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E15" s="86">
-        <f>$H$10*COS(RADIANS(180 - B15)) + $H$4 + $H$10</f>
+        <f t="shared" si="2"/>
         <v>4.5499999999999989</v>
       </c>
-      <c r="I15" s="105"/>
+      <c r="I15" s="90"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="76">
         <v>65</v>
       </c>
       <c r="C16" s="70">
-        <f>$H$11*SIN(RADIANS(180 - B16)) + $H$2</f>
+        <f t="shared" si="0"/>
         <v>7.6252311481466002</v>
       </c>
       <c r="D16" s="70">
-        <f>$H$12 * SIN(RADIANS(B16)) + $H$3</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E16" s="86">
-        <f>$H$10*COS(RADIANS(180 - B16)) + $H$4 + $H$10</f>
+        <f t="shared" si="2"/>
         <v>4.016066006010826</v>
       </c>
     </row>
@@ -5267,15 +5269,15 @@
         <v>70</v>
       </c>
       <c r="C17" s="70">
-        <f>$H$11*SIN(RADIANS(180 - B17)) + $H$2</f>
+        <f t="shared" si="0"/>
         <v>7.7587704831436337</v>
       </c>
       <c r="D17" s="70">
-        <f>$H$12 * SIN(RADIANS(B17)) + $H$3</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E17" s="86">
-        <f>$H$10*COS(RADIANS(180 - B17)) + $H$4 + $H$10</f>
+        <f t="shared" si="2"/>
         <v>3.4599389889471137</v>
       </c>
     </row>
@@ -5284,15 +5286,15 @@
         <v>75</v>
       </c>
       <c r="C18" s="70">
-        <f>$H$11*SIN(RADIANS(180 - B18)) + $H$2</f>
+        <f t="shared" si="0"/>
         <v>7.8637033051562728</v>
       </c>
       <c r="D18" s="70">
-        <f>$H$12 * SIN(RADIANS(B18)) + $H$3</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E18" s="86">
-        <f>$H$10*COS(RADIANS(180 - B18)) + $H$4 + $H$10</f>
+        <f t="shared" si="2"/>
         <v>2.8858514112073941</v>
       </c>
     </row>
@@ -5301,15 +5303,15 @@
         <v>80</v>
       </c>
       <c r="C19" s="70">
-        <f>$H$11*SIN(RADIANS(180 - B19)) + $H$2</f>
+        <f t="shared" si="0"/>
         <v>7.9392310120488325</v>
       </c>
       <c r="D19" s="70">
-        <f>$H$12 * SIN(RADIANS(B19)) + $H$3</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E19" s="86">
-        <f>$H$10*COS(RADIANS(180 - B19)) + $H$4 + $H$10</f>
+        <f t="shared" si="2"/>
         <v>2.2981724259018197</v>
       </c>
     </row>
@@ -5318,15 +5320,15 @@
         <v>85</v>
       </c>
       <c r="C20" s="70">
-        <f>$H$11*SIN(RADIANS(180 - B20)) + $H$2</f>
+        <f t="shared" si="0"/>
         <v>7.9847787923669822</v>
       </c>
       <c r="D20" s="70">
-        <f>$H$12 * SIN(RADIANS(B20)) + $H$3</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E20" s="86">
-        <f>$H$10*COS(RADIANS(180 - B20)) + $H$4 + $H$10</f>
+        <f t="shared" si="2"/>
         <v>1.7013746249588415</v>
       </c>
     </row>
@@ -5335,15 +5337,15 @@
         <v>90</v>
       </c>
       <c r="C21" s="70">
-        <f>$H$11*SIN(RADIANS(180 - B21)) + $H$2</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="D21" s="70">
-        <f>$H$12 * SIN(RADIANS(B21)) + $H$3</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E21" s="86">
-        <f>$H$10*COS(RADIANS(180 - B21)) + $H$4 + $H$10</f>
+        <f t="shared" si="2"/>
         <v>1.0999999999999996</v>
       </c>
     </row>
@@ -5352,15 +5354,15 @@
         <v>95</v>
       </c>
       <c r="C22" s="70">
-        <f>$H$11*SIN(RADIANS(180 - B22)) + $H$2</f>
+        <f t="shared" si="0"/>
         <v>7.9847787923669822</v>
       </c>
       <c r="D22" s="70">
-        <f>$H$12 * SIN(RADIANS(B22)) + $H$3</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E22" s="86">
-        <f>$H$10*COS(RADIANS(180 - B22)) + $H$4 + $H$10</f>
+        <f t="shared" si="2"/>
         <v>0.49862537504115867</v>
       </c>
     </row>
@@ -5369,15 +5371,15 @@
         <v>100</v>
       </c>
       <c r="C23" s="70">
-        <f>$H$11*SIN(RADIANS(180 - B23)) + $H$2</f>
+        <f t="shared" si="0"/>
         <v>7.9392310120488325</v>
       </c>
       <c r="D23" s="70">
-        <f>$H$12 * SIN(RADIANS(B23)) + $H$3</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E23" s="86">
-        <f>$H$10*COS(RADIANS(180 - B23)) + $H$4 + $H$10</f>
+        <f t="shared" si="2"/>
         <v>-9.8172425901820404E-2</v>
       </c>
     </row>
@@ -5386,15 +5388,15 @@
         <v>105</v>
       </c>
       <c r="C24" s="70">
-        <f>$H$11*SIN(RADIANS(180 - B24)) + $H$2</f>
+        <f t="shared" si="0"/>
         <v>7.8637033051562728</v>
       </c>
       <c r="D24" s="70">
-        <f>$H$12 * SIN(RADIANS(B24)) + $H$3</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E24" s="86">
-        <f>$H$10*COS(RADIANS(180 - B24)) + $H$4 + $H$10</f>
+        <f t="shared" si="2"/>
         <v>-0.68585141120739301</v>
       </c>
       <c r="G24" s="68"/>
@@ -5404,15 +5406,15 @@
         <v>110</v>
       </c>
       <c r="C25" s="70">
-        <f>$H$11*SIN(RADIANS(180 - B25)) + $H$2</f>
+        <f t="shared" si="0"/>
         <v>7.7587704831436337</v>
       </c>
       <c r="D25" s="70">
-        <f>$H$12 * SIN(RADIANS(B25)) + $H$3</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E25" s="86">
-        <f>$H$10*COS(RADIANS(180 - B25)) + $H$4 + $H$10</f>
+        <f t="shared" si="2"/>
         <v>-1.2599389889471153</v>
       </c>
     </row>
@@ -5421,15 +5423,15 @@
         <v>115</v>
       </c>
       <c r="C26" s="70">
-        <f>$H$11*SIN(RADIANS(180 - B26)) + $H$2</f>
+        <f t="shared" si="0"/>
         <v>7.6252311481466002</v>
       </c>
       <c r="D26" s="70">
-        <f>$H$12 * SIN(RADIANS(B26)) + $H$3</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E26" s="86">
-        <f>$H$10*COS(RADIANS(180 - B26)) + $H$4 + $H$10</f>
+        <f t="shared" si="2"/>
         <v>-1.8160660060108267</v>
       </c>
     </row>
@@ -5438,15 +5440,15 @@
         <v>120</v>
       </c>
       <c r="C27" s="70">
-        <f>$H$11*SIN(RADIANS(180 - B27)) + $H$2</f>
+        <f t="shared" si="0"/>
         <v>7.4641016151377544</v>
       </c>
       <c r="D27" s="70">
-        <f>$H$12 * SIN(RADIANS(B27)) + $H$3</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E27" s="86">
-        <f>$H$10*COS(RADIANS(180 - B27)) + $H$4 + $H$10</f>
+        <f t="shared" si="2"/>
         <v>-2.3500000000000014</v>
       </c>
     </row>
@@ -5455,15 +5457,15 @@
         <v>125</v>
       </c>
       <c r="C28" s="70">
-        <f>$H$11*SIN(RADIANS(180 - B28)) + $H$2</f>
+        <f t="shared" si="0"/>
         <v>7.2766081771559676</v>
       </c>
       <c r="D28" s="70">
-        <f>$H$12 * SIN(RADIANS(B28)) + $H$3</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E28" s="86">
-        <f>$H$10*COS(RADIANS(180 - B28)) + $H$4 + $H$10</f>
+        <f t="shared" si="2"/>
         <v>-2.8576774108222196</v>
       </c>
     </row>
@@ -5472,15 +5474,15 @@
         <v>130</v>
       </c>
       <c r="C29" s="70">
-        <f>$H$11*SIN(RADIANS(180 - B29)) + $H$2</f>
+        <f t="shared" si="0"/>
         <v>7.0641777724759116</v>
       </c>
       <c r="D29" s="70">
-        <f>$H$12 * SIN(RADIANS(B29)) + $H$3</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E29" s="86">
-        <f>$H$10*COS(RADIANS(180 - B29)) + $H$4 + $H$10</f>
+        <f t="shared" si="2"/>
         <v>-3.3352345068371223</v>
       </c>
     </row>
@@ -5489,15 +5491,15 @@
         <v>135</v>
       </c>
       <c r="C30" s="70">
-        <f>$H$11*SIN(RADIANS(180 - B30)) + $H$2</f>
+        <f t="shared" si="0"/>
         <v>6.8284271247461898</v>
       </c>
       <c r="D30" s="70">
-        <f>$H$12 * SIN(RADIANS(B30)) + $H$3</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E30" s="86">
-        <f>$H$10*COS(RADIANS(180 - B30)) + $H$4 + $H$10</f>
+        <f t="shared" si="2"/>
         <v>-3.7790367901871784</v>
       </c>
     </row>
@@ -5506,15 +5508,15 @@
         <v>140</v>
       </c>
       <c r="C31" s="70">
-        <f>$H$11*SIN(RADIANS(180 - B31)) + $H$2</f>
+        <f t="shared" si="0"/>
         <v>6.571150438746157</v>
       </c>
       <c r="D31" s="70">
-        <f>$H$12 * SIN(RADIANS(B31)) + $H$3</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E31" s="86">
-        <f>$H$10*COS(RADIANS(180 - B31)) + $H$4 + $H$10</f>
+        <f t="shared" si="2"/>
         <v>-4.1857066575209485</v>
       </c>
     </row>
@@ -5523,15 +5525,15 @@
         <v>145</v>
       </c>
       <c r="C32" s="70">
-        <f>$H$11*SIN(RADIANS(180 - B32)) + $H$2</f>
+        <f t="shared" si="0"/>
         <v>6.2943057454041842</v>
       </c>
       <c r="D32" s="70">
-        <f>$H$12 * SIN(RADIANS(B32)) + $H$3</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E32" s="86">
-        <f>$H$10*COS(RADIANS(180 - B32)) + $H$4 + $H$10</f>
+        <f t="shared" si="2"/>
         <v>-4.5521491055940437</v>
       </c>
     </row>
@@ -5540,15 +5542,15 @@
         <v>150</v>
       </c>
       <c r="C33" s="70">
-        <f>$H$11*SIN(RADIANS(180 - B33)) + $H$2</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="D33" s="70">
-        <f>$H$12 * SIN(RADIANS(B33)) + $H$3</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E33" s="86">
-        <f>$H$10*COS(RADIANS(180 - B33)) + $H$4 + $H$10</f>
+        <f t="shared" si="2"/>
         <v>-4.8755752861126274</v>
       </c>
     </row>
@@ -5557,15 +5559,15 @@
         <v>155</v>
       </c>
       <c r="C34" s="70">
-        <f>$H$11*SIN(RADIANS(180 - B34)) + $H$2</f>
+        <f t="shared" si="0"/>
         <v>5.690473046962798</v>
       </c>
       <c r="D34" s="70">
-        <f>$H$12 * SIN(RADIANS(B34)) + $H$3</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E34" s="86">
-        <f>$H$10*COS(RADIANS(180 - B34)) + $H$4 + $H$10</f>
+        <f t="shared" si="2"/>
         <v>-5.1535237305528856</v>
       </c>
     </row>
@@ -5574,15 +5576,15 @@
         <v>160</v>
       </c>
       <c r="C35" s="70">
-        <f>$H$11*SIN(RADIANS(180 - B35)) + $H$2</f>
+        <f t="shared" si="0"/>
         <v>5.3680805733026746</v>
       </c>
       <c r="D35" s="70">
-        <f>$H$12 * SIN(RADIANS(B35)) + $H$3</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E35" s="86">
-        <f>$H$10*COS(RADIANS(180 - B35)) + $H$4 + $H$10</f>
+        <f t="shared" si="2"/>
         <v>-5.3838790834227686</v>
       </c>
     </row>
@@ -5591,15 +5593,15 @@
         <v>165</v>
       </c>
       <c r="C36" s="70">
-        <f>$H$11*SIN(RADIANS(180 - B36)) + $H$2</f>
+        <f t="shared" si="0"/>
         <v>5.035276180410083</v>
       </c>
       <c r="D36" s="70">
-        <f>$H$12 * SIN(RADIANS(B36)) + $H$3</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E36" s="86">
-        <f>$H$10*COS(RADIANS(180 - B36)) + $H$4 + $H$10</f>
+        <f t="shared" si="2"/>
         <v>-5.564888201394572</v>
       </c>
     </row>
@@ -5608,15 +5610,15 @@
         <v>170</v>
       </c>
       <c r="C37" s="70">
-        <f>$H$11*SIN(RADIANS(180 - B37)) + $H$2</f>
+        <f t="shared" si="0"/>
         <v>4.6945927106677212</v>
       </c>
       <c r="D37" s="70">
-        <f>$H$12 * SIN(RADIANS(B37)) + $H$3</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E37" s="86">
-        <f>$H$10*COS(RADIANS(180 - B37)) + $H$4 + $H$10</f>
+        <f t="shared" si="2"/>
         <v>-5.6951734957842364</v>
       </c>
     </row>
@@ -5625,15 +5627,15 @@
         <v>175</v>
       </c>
       <c r="C38" s="70">
-        <f>$H$11*SIN(RADIANS(180 - B38)) + $H$2</f>
+        <f t="shared" si="0"/>
         <v>4.3486229709906326</v>
       </c>
       <c r="D38" s="70">
-        <f>$H$12 * SIN(RADIANS(B38)) + $H$3</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E38" s="86">
-        <f>$H$10*COS(RADIANS(180 - B38)) + $H$4 + $H$10</f>
+        <f t="shared" si="2"/>
         <v>-5.773743416833045</v>
       </c>
     </row>
@@ -5642,15 +5644,15 @@
         <v>180</v>
       </c>
       <c r="C39" s="70">
-        <f>$H$11*SIN(RADIANS(180 - B39)) + $H$2</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="D39" s="70">
-        <f>$H$12 * SIN(RADIANS(B39)) + $H$3</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E39" s="86">
-        <f>$H$10*COS(RADIANS(180 - B39)) + $H$4 + $H$10</f>
+        <f t="shared" si="2"/>
         <v>-5.8000000000000007</v>
       </c>
     </row>

</xml_diff>